<commit_message>
update to recent fw
</commit_message>
<xml_diff>
--- a/index_coop/202206.xlsx
+++ b/index_coop/202206.xlsx
@@ -558,16 +558,16 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>4203.9</v>
+        <v>723.3</v>
       </c>
       <c r="D8">
-        <v>2522.3</v>
+        <v>434</v>
       </c>
       <c r="E8">
-        <v>85209.8</v>
+        <v>81729.3</v>
       </c>
       <c r="F8">
-        <v>56473.7</v>
+        <v>54385.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>